<commit_message>
setting TransactionItem data type to String instead of QueueItem, SMTP_Credential
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="53">
   <si>
     <t>Name</t>
   </si>
@@ -177,6 +177,9 @@
   </si>
   <si>
     <t>GenerateYearlyDispatcherQueue</t>
+  </si>
+  <si>
+    <t>SMTP_Credential</t>
   </si>
 </sst>
 </file>
@@ -511,7 +514,7 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -596,7 +599,14 @@
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8" t="s">
+        <v>52</v>
+      </c>
+    </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>